<commit_message>
update code KSM007(Print_excel) ver 2
</commit_message>
<xml_diff>
--- a/nts.uk/uk.com/com.file/nts.uk.file.com.infra/src/main/resources/report/KSM007.xlsx
+++ b/nts.uk/uk.com/com.file/nts.uk.file.com.infra/src/main/resources/report/KSM007.xlsx
@@ -103,7 +103,7 @@
     <definedName name="PG単価">[6]明細合計!#REF!</definedName>
     <definedName name="PG田中" localSheetId="0">#REF!</definedName>
     <definedName name="PG田中">#REF!</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">帳票テンプレート!$1:$2</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">帳票テンプレート!$1:$1</definedName>
     <definedName name="PrintDaicho" localSheetId="0">[7]!PrintDaicho</definedName>
     <definedName name="PrintDaicho">[7]!PrintDaicho</definedName>
     <definedName name="QuitDaicho" localSheetId="0">[7]!QuitDaicho</definedName>
@@ -233,7 +233,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>&amp;=item.workplaceCode</t>
   </si>
@@ -252,9 +252,6 @@
   <si>
     <t>&amp;=$headerC</t>
   </si>
-  <si>
-    <t>&amp;=$dateTime</t>
-  </si>
 </sst>
 </file>
 
@@ -269,18 +266,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color theme="1"/>
-      <name val="ＭＳ ゴシック"/>
-      <family val="3"/>
-      <charset val="128"/>
-    </font>
-    <font>
       <sz val="6"/>
       <name val="Calibri"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color theme="1"/>
+      <name val="ＭＳ ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
     </font>
   </fonts>
   <fills count="3">
@@ -324,16 +321,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2102,7 +2105,7 @@
             <v>型番</v>
           </cell>
           <cell r="D2" t="str">
-            <v xml:space="preserve">製品名 </v>
+            <v>製品名</v>
           </cell>
           <cell r="E2" t="str">
             <v>仕様</v>
@@ -23683,7 +23686,7 @@
             <v>ACW-CD-S</v>
           </cell>
           <cell r="C140" t="str">
-            <v xml:space="preserve">M6754-5 </v>
+            <v>M6754-5</v>
           </cell>
           <cell r="D140" t="str">
             <v>内蔵CD-ROM装置</v>
@@ -40859,7 +40862,7 @@
             <v>1</v>
           </cell>
           <cell r="E170" t="str">
-            <v xml:space="preserve">'0':未処理、'1':仮処理、'2':本処理、'3':出力不要 </v>
+            <v>'0':未処理、'1':仮処理、'2':本処理、'3':出力不要</v>
           </cell>
         </row>
         <row r="171">
@@ -43944,59 +43947,232 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:CJ2"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScale="190" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" zoomScalePageLayoutView="190" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScale="175" zoomScaleNormal="235" zoomScaleSheetLayoutView="115" zoomScalePageLayoutView="175" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="11.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="19.7" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="27.85546875" style="4" customWidth="1"/>
-    <col min="2" max="2" width="33.42578125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="28.85546875" style="4" customWidth="1"/>
-    <col min="4" max="16384" width="9" style="1"/>
+    <col min="1" max="13" width="2.42578125" style="6" customWidth="1"/>
+    <col min="14" max="58" width="2.42578125" style="3" customWidth="1"/>
+    <col min="59" max="88" width="0.85546875" style="3" customWidth="1"/>
+    <col min="89" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="20.100000000000001" customHeight="1">
-      <c r="A2" s="2" t="s">
+    <row r="1" spans="1:88" ht="19.7" customHeight="1">
+      <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
+      <c r="AA1" s="1"/>
+      <c r="AB1" s="1"/>
+      <c r="AC1" s="1"/>
+      <c r="AD1" s="1"/>
+      <c r="AE1" s="1"/>
+      <c r="AF1" s="1"/>
+      <c r="AG1" s="1"/>
+      <c r="AH1" s="1"/>
+      <c r="AI1" s="1"/>
+      <c r="AJ1" s="1"/>
+      <c r="AK1" s="1"/>
+      <c r="AL1" s="1"/>
+      <c r="AM1" s="2"/>
+      <c r="AN1" s="2"/>
+      <c r="AO1" s="2"/>
+      <c r="AP1" s="2"/>
+      <c r="AQ1" s="2"/>
+      <c r="AR1" s="2"/>
+      <c r="AS1" s="2"/>
+      <c r="AT1" s="2"/>
+      <c r="AU1" s="2"/>
+      <c r="AV1" s="2"/>
+      <c r="AW1" s="2"/>
+      <c r="AX1" s="2"/>
+      <c r="AY1" s="2"/>
+      <c r="AZ1" s="2"/>
+      <c r="BA1" s="2"/>
+      <c r="BB1" s="2"/>
+      <c r="BC1" s="2"/>
+      <c r="BD1" s="2"/>
+      <c r="BE1" s="2"/>
+      <c r="BF1" s="2"/>
+      <c r="BG1" s="2"/>
+      <c r="BH1" s="2"/>
+      <c r="BI1" s="2"/>
+      <c r="BJ1" s="2"/>
+      <c r="BK1" s="2"/>
+      <c r="BL1" s="2"/>
+      <c r="BM1" s="2"/>
+      <c r="BN1" s="2"/>
+      <c r="BO1" s="2"/>
+      <c r="BP1" s="2"/>
+      <c r="BQ1" s="2"/>
+      <c r="BR1" s="2"/>
+      <c r="BS1" s="2"/>
+      <c r="BT1" s="2"/>
+      <c r="BU1" s="2"/>
+      <c r="BV1" s="2"/>
+      <c r="BW1" s="2"/>
+      <c r="BX1" s="2"/>
+      <c r="BY1" s="2"/>
+      <c r="BZ1" s="2"/>
+      <c r="CA1" s="2"/>
+      <c r="CB1" s="2"/>
+      <c r="CC1" s="2"/>
+      <c r="CD1" s="2"/>
+      <c r="CE1" s="2"/>
+      <c r="CF1" s="2"/>
+      <c r="CG1" s="2"/>
+      <c r="CH1" s="2"/>
+      <c r="CI1" s="2"/>
+      <c r="CJ1" s="2"/>
     </row>
-    <row r="3" spans="1:3" ht="31.5" customHeight="1">
-      <c r="A3" s="3" t="s">
+    <row r="2" spans="1:88" ht="19.7" customHeight="1">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4" t="s">
         <v>2</v>
       </c>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="4"/>
+      <c r="T2" s="4"/>
+      <c r="U2" s="4"/>
+      <c r="V2" s="4"/>
+      <c r="W2" s="4"/>
+      <c r="X2" s="4"/>
+      <c r="Y2" s="4"/>
+      <c r="Z2" s="4"/>
+      <c r="AA2" s="4"/>
+      <c r="AB2" s="4"/>
+      <c r="AC2" s="4"/>
+      <c r="AD2" s="4"/>
+      <c r="AE2" s="4"/>
+      <c r="AF2" s="4"/>
+      <c r="AG2" s="4"/>
+      <c r="AH2" s="4"/>
+      <c r="AI2" s="4"/>
+      <c r="AJ2" s="4"/>
+      <c r="AK2" s="4"/>
+      <c r="AL2" s="4"/>
+      <c r="AM2" s="5"/>
+      <c r="AN2" s="5"/>
+      <c r="AO2" s="5"/>
+      <c r="AP2" s="5"/>
+      <c r="AQ2" s="5"/>
+      <c r="AR2" s="5"/>
+      <c r="AS2" s="5"/>
+      <c r="AT2" s="5"/>
+      <c r="AU2" s="5"/>
+      <c r="AV2" s="5"/>
+      <c r="AW2" s="5"/>
+      <c r="AX2" s="5"/>
+      <c r="AY2" s="5"/>
+      <c r="AZ2" s="5"/>
+      <c r="BA2" s="5"/>
+      <c r="BB2" s="5"/>
+      <c r="BC2" s="5"/>
+      <c r="BD2" s="5"/>
+      <c r="BE2" s="5"/>
+      <c r="BF2" s="5"/>
+      <c r="BG2" s="5"/>
+      <c r="BH2" s="5"/>
+      <c r="BI2" s="5"/>
+      <c r="BJ2" s="5"/>
+      <c r="BK2" s="5"/>
+      <c r="BL2" s="5"/>
+      <c r="BM2" s="5"/>
+      <c r="BN2" s="5"/>
+      <c r="BO2" s="5"/>
+      <c r="BP2" s="5"/>
+      <c r="BQ2" s="5"/>
+      <c r="BR2" s="5"/>
+      <c r="BS2" s="5"/>
+      <c r="BT2" s="5"/>
+      <c r="BU2" s="5"/>
+      <c r="BV2" s="5"/>
+      <c r="BW2" s="5"/>
+      <c r="BX2" s="5"/>
+      <c r="BY2" s="5"/>
+      <c r="BZ2" s="5"/>
+      <c r="CA2" s="5"/>
+      <c r="CB2" s="5"/>
+      <c r="CC2" s="5"/>
+      <c r="CD2" s="5"/>
+      <c r="CE2" s="5"/>
+      <c r="CF2" s="5"/>
+      <c r="CG2" s="5"/>
+      <c r="CH2" s="5"/>
+      <c r="CI2" s="5"/>
+      <c r="CJ2" s="5"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="2"/>
-  <conditionalFormatting sqref="A3:XFD70">
+  <mergeCells count="6">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="E1:L1"/>
+    <mergeCell ref="E2:L2"/>
+    <mergeCell ref="M1:AL1"/>
+    <mergeCell ref="M2:AL2"/>
+  </mergeCells>
+  <phoneticPr fontId="1"/>
+  <conditionalFormatting sqref="A2 E2 M2 CK2:XFD69 A3:CJ69">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions horizontalCentered="1"/>
-  <pageMargins left="0.39370078740157499" right="0.39370078740157499" top="0.98425196850393704" bottom="0.39370078740157499" header="0.39370078740157499" footer="0.31496062992126"/>
+  <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.98425196850393704" bottom="0.39370078740157483" header="0.39370078740157483" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter>
-    <oddHeader xml:space="preserve">&amp;L&amp;"ＭＳ ゴシック,標準"&amp;9&amp;=$companyName&amp;C&amp;"ＭＳ ゴシック,標準"&amp;16&amp;=titleName(bean)&amp;R&amp;"ＭＳ ゴシック,標準"&amp;9&amp;D　&amp;T　
+    <oddHeader xml:space="preserve">&amp;L&amp;"ＭＳ ゴシック,標準"&amp;8&amp;=$companyName&amp;C&amp;"ＭＳ ゴシック,標準"&amp;14&amp;=titleName(bean)&amp;R&amp;"ＭＳ ゴシック,標準"&amp;8&amp;D　&amp;T　
 page&amp;P
 </oddHeader>
     <firstHeader>&amp;L日通システム株式会社&amp;Cアラームリスト(個人別)&amp;R2017/11/15  14:49:00

</xml_diff>

<commit_message>
move ksm007 to at context
</commit_message>
<xml_diff>
--- a/nts.uk/uk.com/com.file/nts.uk.file.com.infra/src/main/resources/report/KSM007.xlsx
+++ b/nts.uk/uk.com/com.file/nts.uk.file.com.infra/src/main/resources/report/KSM007.xlsx
@@ -273,7 +273,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="7"/>
+      <sz val="8"/>
       <color theme="1"/>
       <name val="ＭＳ ゴシック"/>
       <family val="3"/>
@@ -294,7 +294,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -317,28 +317,158 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -43947,230 +44077,247 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CJ2"/>
+  <dimension ref="A1:CO2"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScale="175" zoomScaleNormal="235" zoomScaleSheetLayoutView="115" zoomScalePageLayoutView="175" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScale="160" zoomScaleNormal="235" zoomScaleSheetLayoutView="115" zoomScalePageLayoutView="160" workbookViewId="0">
+      <selection activeCell="AN7" sqref="AN7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="19.7" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.600000000000001" customHeight="1"/>
   <cols>
-    <col min="1" max="13" width="2.42578125" style="6" customWidth="1"/>
-    <col min="14" max="58" width="2.42578125" style="3" customWidth="1"/>
-    <col min="59" max="88" width="0.85546875" style="3" customWidth="1"/>
-    <col min="89" max="16384" width="9" style="3"/>
+    <col min="1" max="1" width="2.42578125" style="19" customWidth="1"/>
+    <col min="2" max="3" width="2.42578125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="2.42578125" style="20" customWidth="1"/>
+    <col min="5" max="16" width="2.42578125" style="4" customWidth="1"/>
+    <col min="17" max="17" width="2.42578125" style="20" customWidth="1"/>
+    <col min="18" max="18" width="2.42578125" style="4" customWidth="1"/>
+    <col min="19" max="56" width="2.42578125" style="2" customWidth="1"/>
+    <col min="57" max="57" width="2.42578125" style="21" customWidth="1"/>
+    <col min="58" max="63" width="2.42578125" style="2" customWidth="1"/>
+    <col min="64" max="93" width="0.85546875" style="2" customWidth="1"/>
+    <col min="94" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:88" ht="19.7" customHeight="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:93" ht="18.600000000000001" customHeight="1">
+      <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1" t="s">
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1" t="s">
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
-      <c r="Y1" s="1"/>
-      <c r="Z1" s="1"/>
-      <c r="AA1" s="1"/>
-      <c r="AB1" s="1"/>
-      <c r="AC1" s="1"/>
-      <c r="AD1" s="1"/>
-      <c r="AE1" s="1"/>
-      <c r="AF1" s="1"/>
-      <c r="AG1" s="1"/>
-      <c r="AH1" s="1"/>
-      <c r="AI1" s="1"/>
-      <c r="AJ1" s="1"/>
-      <c r="AK1" s="1"/>
-      <c r="AL1" s="1"/>
-      <c r="AM1" s="2"/>
-      <c r="AN1" s="2"/>
-      <c r="AO1" s="2"/>
-      <c r="AP1" s="2"/>
-      <c r="AQ1" s="2"/>
-      <c r="AR1" s="2"/>
-      <c r="AS1" s="2"/>
-      <c r="AT1" s="2"/>
-      <c r="AU1" s="2"/>
-      <c r="AV1" s="2"/>
-      <c r="AW1" s="2"/>
-      <c r="AX1" s="2"/>
-      <c r="AY1" s="2"/>
-      <c r="AZ1" s="2"/>
-      <c r="BA1" s="2"/>
-      <c r="BB1" s="2"/>
-      <c r="BC1" s="2"/>
-      <c r="BD1" s="2"/>
-      <c r="BE1" s="2"/>
-      <c r="BF1" s="2"/>
-      <c r="BG1" s="2"/>
-      <c r="BH1" s="2"/>
-      <c r="BI1" s="2"/>
-      <c r="BJ1" s="2"/>
-      <c r="BK1" s="2"/>
-      <c r="BL1" s="2"/>
-      <c r="BM1" s="2"/>
-      <c r="BN1" s="2"/>
-      <c r="BO1" s="2"/>
-      <c r="BP1" s="2"/>
-      <c r="BQ1" s="2"/>
-      <c r="BR1" s="2"/>
-      <c r="BS1" s="2"/>
-      <c r="BT1" s="2"/>
-      <c r="BU1" s="2"/>
-      <c r="BV1" s="2"/>
-      <c r="BW1" s="2"/>
-      <c r="BX1" s="2"/>
-      <c r="BY1" s="2"/>
-      <c r="BZ1" s="2"/>
-      <c r="CA1" s="2"/>
-      <c r="CB1" s="2"/>
-      <c r="CC1" s="2"/>
-      <c r="CD1" s="2"/>
-      <c r="CE1" s="2"/>
-      <c r="CF1" s="2"/>
-      <c r="CG1" s="2"/>
-      <c r="CH1" s="2"/>
-      <c r="CI1" s="2"/>
-      <c r="CJ1" s="2"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
+      <c r="V1" s="6"/>
+      <c r="W1" s="6"/>
+      <c r="X1" s="6"/>
+      <c r="Y1" s="6"/>
+      <c r="Z1" s="6"/>
+      <c r="AA1" s="6"/>
+      <c r="AB1" s="6"/>
+      <c r="AC1" s="6"/>
+      <c r="AD1" s="6"/>
+      <c r="AE1" s="6"/>
+      <c r="AF1" s="6"/>
+      <c r="AG1" s="6"/>
+      <c r="AH1" s="6"/>
+      <c r="AI1" s="6"/>
+      <c r="AJ1" s="6"/>
+      <c r="AK1" s="6"/>
+      <c r="AL1" s="6"/>
+      <c r="AM1" s="6"/>
+      <c r="AN1" s="6"/>
+      <c r="AO1" s="6"/>
+      <c r="AP1" s="6"/>
+      <c r="AQ1" s="6"/>
+      <c r="AR1" s="6"/>
+      <c r="AS1" s="6"/>
+      <c r="AT1" s="6"/>
+      <c r="AU1" s="6"/>
+      <c r="AV1" s="6"/>
+      <c r="AW1" s="6"/>
+      <c r="AX1" s="6"/>
+      <c r="AY1" s="6"/>
+      <c r="AZ1" s="6"/>
+      <c r="BA1" s="6"/>
+      <c r="BB1" s="6"/>
+      <c r="BC1" s="6"/>
+      <c r="BD1" s="6"/>
+      <c r="BE1" s="17"/>
+      <c r="BF1" s="1"/>
+      <c r="BG1" s="1"/>
+      <c r="BH1" s="1"/>
+      <c r="BI1" s="1"/>
+      <c r="BJ1" s="1"/>
+      <c r="BK1" s="1"/>
+      <c r="BL1" s="1"/>
+      <c r="BM1" s="1"/>
+      <c r="BN1" s="1"/>
+      <c r="BO1" s="1"/>
+      <c r="BP1" s="1"/>
+      <c r="BQ1" s="1"/>
+      <c r="BR1" s="1"/>
+      <c r="BS1" s="1"/>
+      <c r="BT1" s="1"/>
+      <c r="BU1" s="1"/>
+      <c r="BV1" s="1"/>
+      <c r="BW1" s="1"/>
+      <c r="BX1" s="1"/>
+      <c r="BY1" s="1"/>
+      <c r="BZ1" s="1"/>
+      <c r="CA1" s="1"/>
+      <c r="CB1" s="1"/>
+      <c r="CC1" s="1"/>
+      <c r="CD1" s="1"/>
+      <c r="CE1" s="1"/>
+      <c r="CF1" s="1"/>
+      <c r="CG1" s="1"/>
+      <c r="CH1" s="1"/>
+      <c r="CI1" s="1"/>
+      <c r="CJ1" s="1"/>
+      <c r="CK1" s="1"/>
+      <c r="CL1" s="1"/>
+      <c r="CM1" s="1"/>
+      <c r="CN1" s="1"/>
+      <c r="CO1" s="1"/>
     </row>
-    <row r="2" spans="1:88" ht="19.7" customHeight="1">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:93" ht="18.600000000000001" customHeight="1">
+      <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4" t="s">
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4" t="s">
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="16"/>
+      <c r="R2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="4"/>
-      <c r="T2" s="4"/>
-      <c r="U2" s="4"/>
-      <c r="V2" s="4"/>
-      <c r="W2" s="4"/>
-      <c r="X2" s="4"/>
-      <c r="Y2" s="4"/>
-      <c r="Z2" s="4"/>
-      <c r="AA2" s="4"/>
-      <c r="AB2" s="4"/>
-      <c r="AC2" s="4"/>
-      <c r="AD2" s="4"/>
-      <c r="AE2" s="4"/>
-      <c r="AF2" s="4"/>
-      <c r="AG2" s="4"/>
-      <c r="AH2" s="4"/>
-      <c r="AI2" s="4"/>
-      <c r="AJ2" s="4"/>
-      <c r="AK2" s="4"/>
-      <c r="AL2" s="4"/>
-      <c r="AM2" s="5"/>
-      <c r="AN2" s="5"/>
-      <c r="AO2" s="5"/>
-      <c r="AP2" s="5"/>
-      <c r="AQ2" s="5"/>
-      <c r="AR2" s="5"/>
-      <c r="AS2" s="5"/>
-      <c r="AT2" s="5"/>
-      <c r="AU2" s="5"/>
-      <c r="AV2" s="5"/>
-      <c r="AW2" s="5"/>
-      <c r="AX2" s="5"/>
-      <c r="AY2" s="5"/>
-      <c r="AZ2" s="5"/>
-      <c r="BA2" s="5"/>
-      <c r="BB2" s="5"/>
-      <c r="BC2" s="5"/>
-      <c r="BD2" s="5"/>
-      <c r="BE2" s="5"/>
-      <c r="BF2" s="5"/>
-      <c r="BG2" s="5"/>
-      <c r="BH2" s="5"/>
-      <c r="BI2" s="5"/>
-      <c r="BJ2" s="5"/>
-      <c r="BK2" s="5"/>
-      <c r="BL2" s="5"/>
-      <c r="BM2" s="5"/>
-      <c r="BN2" s="5"/>
-      <c r="BO2" s="5"/>
-      <c r="BP2" s="5"/>
-      <c r="BQ2" s="5"/>
-      <c r="BR2" s="5"/>
-      <c r="BS2" s="5"/>
-      <c r="BT2" s="5"/>
-      <c r="BU2" s="5"/>
-      <c r="BV2" s="5"/>
-      <c r="BW2" s="5"/>
-      <c r="BX2" s="5"/>
-      <c r="BY2" s="5"/>
-      <c r="BZ2" s="5"/>
-      <c r="CA2" s="5"/>
-      <c r="CB2" s="5"/>
-      <c r="CC2" s="5"/>
-      <c r="CD2" s="5"/>
-      <c r="CE2" s="5"/>
-      <c r="CF2" s="5"/>
-      <c r="CG2" s="5"/>
-      <c r="CH2" s="5"/>
-      <c r="CI2" s="5"/>
-      <c r="CJ2" s="5"/>
+      <c r="S2" s="9"/>
+      <c r="T2" s="9"/>
+      <c r="U2" s="9"/>
+      <c r="V2" s="9"/>
+      <c r="W2" s="9"/>
+      <c r="X2" s="9"/>
+      <c r="Y2" s="9"/>
+      <c r="Z2" s="9"/>
+      <c r="AA2" s="9"/>
+      <c r="AB2" s="9"/>
+      <c r="AC2" s="9"/>
+      <c r="AD2" s="9"/>
+      <c r="AE2" s="9"/>
+      <c r="AF2" s="9"/>
+      <c r="AG2" s="9"/>
+      <c r="AH2" s="9"/>
+      <c r="AI2" s="9"/>
+      <c r="AJ2" s="9"/>
+      <c r="AK2" s="9"/>
+      <c r="AL2" s="9"/>
+      <c r="AM2" s="9"/>
+      <c r="AN2" s="9"/>
+      <c r="AO2" s="9"/>
+      <c r="AP2" s="9"/>
+      <c r="AQ2" s="9"/>
+      <c r="AR2" s="9"/>
+      <c r="AS2" s="9"/>
+      <c r="AT2" s="9"/>
+      <c r="AU2" s="9"/>
+      <c r="AV2" s="9"/>
+      <c r="AW2" s="9"/>
+      <c r="AX2" s="9"/>
+      <c r="AY2" s="9"/>
+      <c r="AZ2" s="9"/>
+      <c r="BA2" s="9"/>
+      <c r="BB2" s="9"/>
+      <c r="BC2" s="9"/>
+      <c r="BD2" s="9"/>
+      <c r="BE2" s="18"/>
+      <c r="BF2" s="3"/>
+      <c r="BG2" s="3"/>
+      <c r="BH2" s="3"/>
+      <c r="BI2" s="3"/>
+      <c r="BJ2" s="3"/>
+      <c r="BK2" s="3"/>
+      <c r="BL2" s="3"/>
+      <c r="BM2" s="3"/>
+      <c r="BN2" s="3"/>
+      <c r="BO2" s="3"/>
+      <c r="BP2" s="3"/>
+      <c r="BQ2" s="3"/>
+      <c r="BR2" s="3"/>
+      <c r="BS2" s="3"/>
+      <c r="BT2" s="3"/>
+      <c r="BU2" s="3"/>
+      <c r="BV2" s="3"/>
+      <c r="BW2" s="3"/>
+      <c r="BX2" s="3"/>
+      <c r="BY2" s="3"/>
+      <c r="BZ2" s="3"/>
+      <c r="CA2" s="3"/>
+      <c r="CB2" s="3"/>
+      <c r="CC2" s="3"/>
+      <c r="CD2" s="3"/>
+      <c r="CE2" s="3"/>
+      <c r="CF2" s="3"/>
+      <c r="CG2" s="3"/>
+      <c r="CH2" s="3"/>
+      <c r="CI2" s="3"/>
+      <c r="CJ2" s="3"/>
+      <c r="CK2" s="3"/>
+      <c r="CL2" s="3"/>
+      <c r="CM2" s="3"/>
+      <c r="CN2" s="3"/>
+      <c r="CO2" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A2:D2"/>
-    <mergeCell ref="E1:L1"/>
-    <mergeCell ref="E2:L2"/>
-    <mergeCell ref="M1:AL1"/>
-    <mergeCell ref="M2:AL2"/>
+    <mergeCell ref="E1:Q1"/>
+    <mergeCell ref="E2:Q2"/>
+    <mergeCell ref="R1:BE1"/>
+    <mergeCell ref="R2:BE2"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
-  <conditionalFormatting sqref="A2 E2 M2 CK2:XFD69 A3:CJ69">
+  <conditionalFormatting sqref="A2 E2 R2 CP2:XFD69 A3:CO69">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions horizontalCentered="1"/>
-  <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.98425196850393704" bottom="0.39370078740157483" header="0.39370078740157483" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.39370078740157499" right="0.39370078740157499" top="0.98425196850393704" bottom="0.39370078740157499" header="0.39370078740157499" footer="0.31496062992126"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddHeader xml:space="preserve">&amp;L&amp;"ＭＳ ゴシック,標準"&amp;8&amp;=$companyName&amp;C&amp;"ＭＳ ゴシック,標準"&amp;14&amp;=titleName(bean)&amp;R&amp;"ＭＳ ゴシック,標準"&amp;8&amp;D　&amp;T　
 page&amp;P

</xml_diff>

<commit_message>
fix bugs after test
</commit_message>
<xml_diff>
--- a/nts.uk/uk.com/com.file/nts.uk.file.com.infra/src/main/resources/report/KSM007.xlsx
+++ b/nts.uk/uk.com/com.file/nts.uk.file.com.infra/src/main/resources/report/KSM007.xlsx
@@ -294,12 +294,43 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="16">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -309,59 +340,7 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="dotted">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -374,9 +353,7 @@
       <right style="dotted">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -387,9 +364,16 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top style="thin">
+      <top/>
+      <bottom style="thin">
         <color indexed="64"/>
-      </top>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -401,7 +385,102 @@
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -420,55 +499,55 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -44080,88 +44159,88 @@
   <dimension ref="A1:CO2"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScale="160" zoomScaleNormal="235" zoomScaleSheetLayoutView="115" zoomScalePageLayoutView="160" workbookViewId="0">
-      <selection activeCell="AN7" sqref="AN7"/>
+      <selection activeCell="AG8" sqref="AG8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.600000000000001" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="2.42578125" style="19" customWidth="1"/>
+    <col min="1" max="1" width="2.42578125" style="5" customWidth="1"/>
     <col min="2" max="3" width="2.42578125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="2.42578125" style="20" customWidth="1"/>
+    <col min="4" max="4" width="2.42578125" style="6" customWidth="1"/>
     <col min="5" max="16" width="2.42578125" style="4" customWidth="1"/>
-    <col min="17" max="17" width="2.42578125" style="20" customWidth="1"/>
+    <col min="17" max="17" width="2.42578125" style="6" customWidth="1"/>
     <col min="18" max="18" width="2.42578125" style="4" customWidth="1"/>
     <col min="19" max="56" width="2.42578125" style="2" customWidth="1"/>
-    <col min="57" max="57" width="2.42578125" style="21" customWidth="1"/>
+    <col min="57" max="57" width="2.42578125" style="7" customWidth="1"/>
     <col min="58" max="63" width="2.42578125" style="2" customWidth="1"/>
     <col min="64" max="93" width="0.85546875" style="2" customWidth="1"/>
     <col min="94" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:93" ht="18.600000000000001" customHeight="1">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:93" ht="18.600000000000001" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="11" t="s">
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12"/>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="5" t="s">
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
+      <c r="P1" s="19"/>
+      <c r="Q1" s="20"/>
+      <c r="R1" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6"/>
-      <c r="U1" s="6"/>
-      <c r="V1" s="6"/>
-      <c r="W1" s="6"/>
-      <c r="X1" s="6"/>
-      <c r="Y1" s="6"/>
-      <c r="Z1" s="6"/>
-      <c r="AA1" s="6"/>
-      <c r="AB1" s="6"/>
-      <c r="AC1" s="6"/>
-      <c r="AD1" s="6"/>
-      <c r="AE1" s="6"/>
-      <c r="AF1" s="6"/>
-      <c r="AG1" s="6"/>
-      <c r="AH1" s="6"/>
-      <c r="AI1" s="6"/>
-      <c r="AJ1" s="6"/>
-      <c r="AK1" s="6"/>
-      <c r="AL1" s="6"/>
-      <c r="AM1" s="6"/>
-      <c r="AN1" s="6"/>
-      <c r="AO1" s="6"/>
-      <c r="AP1" s="6"/>
-      <c r="AQ1" s="6"/>
-      <c r="AR1" s="6"/>
-      <c r="AS1" s="6"/>
-      <c r="AT1" s="6"/>
-      <c r="AU1" s="6"/>
-      <c r="AV1" s="6"/>
-      <c r="AW1" s="6"/>
-      <c r="AX1" s="6"/>
-      <c r="AY1" s="6"/>
-      <c r="AZ1" s="6"/>
-      <c r="BA1" s="6"/>
-      <c r="BB1" s="6"/>
-      <c r="BC1" s="6"/>
-      <c r="BD1" s="6"/>
-      <c r="BE1" s="17"/>
+      <c r="S1" s="16"/>
+      <c r="T1" s="16"/>
+      <c r="U1" s="16"/>
+      <c r="V1" s="16"/>
+      <c r="W1" s="16"/>
+      <c r="X1" s="16"/>
+      <c r="Y1" s="16"/>
+      <c r="Z1" s="16"/>
+      <c r="AA1" s="16"/>
+      <c r="AB1" s="16"/>
+      <c r="AC1" s="16"/>
+      <c r="AD1" s="16"/>
+      <c r="AE1" s="16"/>
+      <c r="AF1" s="16"/>
+      <c r="AG1" s="16"/>
+      <c r="AH1" s="16"/>
+      <c r="AI1" s="16"/>
+      <c r="AJ1" s="16"/>
+      <c r="AK1" s="16"/>
+      <c r="AL1" s="16"/>
+      <c r="AM1" s="16"/>
+      <c r="AN1" s="16"/>
+      <c r="AO1" s="16"/>
+      <c r="AP1" s="16"/>
+      <c r="AQ1" s="16"/>
+      <c r="AR1" s="16"/>
+      <c r="AS1" s="16"/>
+      <c r="AT1" s="16"/>
+      <c r="AU1" s="16"/>
+      <c r="AV1" s="16"/>
+      <c r="AW1" s="16"/>
+      <c r="AX1" s="16"/>
+      <c r="AY1" s="16"/>
+      <c r="AZ1" s="16"/>
+      <c r="BA1" s="16"/>
+      <c r="BB1" s="16"/>
+      <c r="BC1" s="16"/>
+      <c r="BD1" s="16"/>
+      <c r="BE1" s="21"/>
       <c r="BF1" s="1"/>
       <c r="BG1" s="1"/>
       <c r="BH1" s="1"/>
@@ -44199,28 +44278,28 @@
       <c r="CN1" s="1"/>
       <c r="CO1" s="1"/>
     </row>
-    <row r="2" spans="1:93" ht="18.600000000000001" customHeight="1">
+    <row r="2" spans="1:93" ht="18.600000000000001" customHeight="1" thickTop="1">
       <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
       <c r="D2" s="10"/>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
-      <c r="M2" s="15"/>
-      <c r="N2" s="15"/>
-      <c r="O2" s="15"/>
-      <c r="P2" s="15"/>
-      <c r="Q2" s="16"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="12"/>
+      <c r="O2" s="12"/>
+      <c r="P2" s="12"/>
+      <c r="Q2" s="13"/>
       <c r="R2" s="8" t="s">
         <v>2</v>
       </c>
@@ -44262,7 +44341,7 @@
       <c r="BB2" s="9"/>
       <c r="BC2" s="9"/>
       <c r="BD2" s="9"/>
-      <c r="BE2" s="18"/>
+      <c r="BE2" s="14"/>
       <c r="BF2" s="3"/>
       <c r="BG2" s="3"/>
       <c r="BH2" s="3"/>

</xml_diff>